<commit_message>
update formatting of rubric
</commit_message>
<xml_diff>
--- a/content/docs/other/dprep-project-rubric.xlsx
+++ b/content/docs/other/dprep-project-rubric.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\course-dprep\content\docs\other\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannesdatta/research/course-dprep/content/docs/other/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D415DBA-F213-4206-8937-530780A5F390}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{099E696D-EA93-164F-96F3-5E7FFF3E6576}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="945" yWindow="360" windowWidth="26070" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4340" yWindow="500" windowWidth="24460" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -506,7 +506,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -531,20 +531,33 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -768,18 +781,18 @@
   </sheetPr>
   <dimension ref="A1:Z38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="55" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:Z2"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScaleNormal="100" zoomScaleSheetLayoutView="55" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="48.5703125" customWidth="1"/>
-    <col min="2" max="4" width="42.28515625" customWidth="1"/>
-    <col min="5" max="5" width="25.42578125" customWidth="1"/>
+    <col min="1" max="1" width="48.5" customWidth="1"/>
+    <col min="2" max="4" width="42.33203125" customWidth="1"/>
+    <col min="5" max="5" width="25.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -817,67 +830,67 @@
       <c r="Y1" s="6"/>
       <c r="Z1" s="6"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A2" s="16" t="s">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.15">
+      <c r="A2" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17"/>
-      <c r="M2" s="17"/>
-      <c r="N2" s="17"/>
-      <c r="O2" s="17"/>
-      <c r="P2" s="17"/>
-      <c r="Q2" s="17"/>
-      <c r="R2" s="17"/>
-      <c r="S2" s="17"/>
-      <c r="T2" s="17"/>
-      <c r="U2" s="17"/>
-      <c r="V2" s="17"/>
-      <c r="W2" s="17"/>
-      <c r="X2" s="17"/>
-      <c r="Y2" s="17"/>
-      <c r="Z2" s="17"/>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A3" s="18" t="s">
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
+      <c r="O2" s="13"/>
+      <c r="P2" s="13"/>
+      <c r="Q2" s="13"/>
+      <c r="R2" s="13"/>
+      <c r="S2" s="13"/>
+      <c r="T2" s="13"/>
+      <c r="U2" s="13"/>
+      <c r="V2" s="13"/>
+      <c r="W2" s="13"/>
+      <c r="X2" s="13"/>
+      <c r="Y2" s="13"/>
+      <c r="Z2" s="13"/>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.15">
+      <c r="A3" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="17"/>
-      <c r="M3" s="17"/>
-      <c r="N3" s="17"/>
-      <c r="O3" s="17"/>
-      <c r="P3" s="17"/>
-      <c r="Q3" s="17"/>
-      <c r="R3" s="17"/>
-      <c r="S3" s="17"/>
-      <c r="T3" s="17"/>
-      <c r="U3" s="17"/>
-      <c r="V3" s="17"/>
-      <c r="W3" s="17"/>
-      <c r="X3" s="17"/>
-      <c r="Y3" s="17"/>
-      <c r="Z3" s="17"/>
-    </row>
-    <row r="4" spans="1:26" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13"/>
+      <c r="M3" s="13"/>
+      <c r="N3" s="13"/>
+      <c r="O3" s="13"/>
+      <c r="P3" s="13"/>
+      <c r="Q3" s="13"/>
+      <c r="R3" s="13"/>
+      <c r="S3" s="13"/>
+      <c r="T3" s="13"/>
+      <c r="U3" s="13"/>
+      <c r="V3" s="13"/>
+      <c r="W3" s="13"/>
+      <c r="X3" s="13"/>
+      <c r="Y3" s="13"/>
+      <c r="Z3" s="13"/>
+    </row>
+    <row r="4" spans="1:26" ht="28" x14ac:dyDescent="0.15">
       <c r="A4" s="7" t="s">
         <v>7</v>
       </c>
@@ -890,8 +903,30 @@
       <c r="D4" s="7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:26" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="16"/>
+      <c r="N4" s="16"/>
+      <c r="O4" s="16"/>
+      <c r="P4" s="16"/>
+      <c r="Q4" s="16"/>
+      <c r="R4" s="16"/>
+      <c r="S4" s="16"/>
+      <c r="T4" s="16"/>
+      <c r="U4" s="16"/>
+      <c r="V4" s="16"/>
+      <c r="W4" s="16"/>
+      <c r="X4" s="16"/>
+      <c r="Y4" s="16"/>
+      <c r="Z4" s="16"/>
+    </row>
+    <row r="5" spans="1:26" ht="28" x14ac:dyDescent="0.15">
       <c r="A5" s="7" t="s">
         <v>11</v>
       </c>
@@ -904,8 +939,30 @@
       <c r="D5" s="7" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:26" ht="51" x14ac:dyDescent="0.2">
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="16"/>
+      <c r="M5" s="16"/>
+      <c r="N5" s="16"/>
+      <c r="O5" s="16"/>
+      <c r="P5" s="16"/>
+      <c r="Q5" s="16"/>
+      <c r="R5" s="16"/>
+      <c r="S5" s="16"/>
+      <c r="T5" s="16"/>
+      <c r="U5" s="16"/>
+      <c r="V5" s="16"/>
+      <c r="W5" s="16"/>
+      <c r="X5" s="16"/>
+      <c r="Y5" s="16"/>
+      <c r="Z5" s="16"/>
+    </row>
+    <row r="6" spans="1:26" ht="42" x14ac:dyDescent="0.15">
       <c r="A6" s="7" t="s">
         <v>15</v>
       </c>
@@ -918,8 +975,30 @@
       <c r="D6" s="7" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="7" spans="1:26" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="16"/>
+      <c r="N6" s="16"/>
+      <c r="O6" s="16"/>
+      <c r="P6" s="16"/>
+      <c r="Q6" s="16"/>
+      <c r="R6" s="16"/>
+      <c r="S6" s="16"/>
+      <c r="T6" s="16"/>
+      <c r="U6" s="16"/>
+      <c r="V6" s="16"/>
+      <c r="W6" s="16"/>
+      <c r="X6" s="16"/>
+      <c r="Y6" s="16"/>
+      <c r="Z6" s="16"/>
+    </row>
+    <row r="7" spans="1:26" ht="42" x14ac:dyDescent="0.15">
       <c r="A7" s="7" t="s">
         <v>19</v>
       </c>
@@ -932,9 +1011,31 @@
       <c r="D7" s="7" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A8" s="19" t="s">
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="16"/>
+      <c r="L7" s="16"/>
+      <c r="M7" s="16"/>
+      <c r="N7" s="16"/>
+      <c r="O7" s="16"/>
+      <c r="P7" s="16"/>
+      <c r="Q7" s="16"/>
+      <c r="R7" s="16"/>
+      <c r="S7" s="16"/>
+      <c r="T7" s="16"/>
+      <c r="U7" s="16"/>
+      <c r="V7" s="16"/>
+      <c r="W7" s="16"/>
+      <c r="X7" s="16"/>
+      <c r="Y7" s="16"/>
+      <c r="Z7" s="16"/>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.15">
+      <c r="A8" s="14" t="s">
         <v>23</v>
       </c>
       <c r="B8" s="17"/>
@@ -963,7 +1064,7 @@
       <c r="Y8" s="17"/>
       <c r="Z8" s="17"/>
     </row>
-    <row r="9" spans="1:26" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:26" ht="98" x14ac:dyDescent="0.15">
       <c r="A9" s="8" t="s">
         <v>24</v>
       </c>
@@ -976,30 +1077,30 @@
       <c r="D9" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
-      <c r="N9" s="6"/>
-      <c r="O9" s="6"/>
-      <c r="P9" s="6"/>
-      <c r="Q9" s="6"/>
-      <c r="R9" s="6"/>
-      <c r="S9" s="6"/>
-      <c r="T9" s="6"/>
-      <c r="U9" s="6"/>
-      <c r="V9" s="6"/>
-      <c r="W9" s="6"/>
-      <c r="X9" s="6"/>
-      <c r="Y9" s="6"/>
-      <c r="Z9" s="6"/>
-    </row>
-    <row r="10" spans="1:26" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="8"/>
+      <c r="O9" s="8"/>
+      <c r="P9" s="8"/>
+      <c r="Q9" s="8"/>
+      <c r="R9" s="8"/>
+      <c r="S9" s="8"/>
+      <c r="T9" s="8"/>
+      <c r="U9" s="8"/>
+      <c r="V9" s="8"/>
+      <c r="W9" s="8"/>
+      <c r="X9" s="8"/>
+      <c r="Y9" s="8"/>
+      <c r="Z9" s="8"/>
+    </row>
+    <row r="10" spans="1:26" ht="56" x14ac:dyDescent="0.15">
       <c r="A10" s="8" t="s">
         <v>28</v>
       </c>
@@ -1012,30 +1113,30 @@
       <c r="D10" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="6"/>
-      <c r="O10" s="6"/>
-      <c r="P10" s="6"/>
-      <c r="Q10" s="6"/>
-      <c r="R10" s="6"/>
-      <c r="S10" s="6"/>
-      <c r="T10" s="6"/>
-      <c r="U10" s="6"/>
-      <c r="V10" s="6"/>
-      <c r="W10" s="6"/>
-      <c r="X10" s="6"/>
-      <c r="Y10" s="6"/>
-      <c r="Z10" s="6"/>
-    </row>
-    <row r="11" spans="1:26" ht="51" x14ac:dyDescent="0.2">
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="8"/>
+      <c r="P10" s="8"/>
+      <c r="Q10" s="8"/>
+      <c r="R10" s="8"/>
+      <c r="S10" s="8"/>
+      <c r="T10" s="8"/>
+      <c r="U10" s="8"/>
+      <c r="V10" s="8"/>
+      <c r="W10" s="8"/>
+      <c r="X10" s="8"/>
+      <c r="Y10" s="8"/>
+      <c r="Z10" s="8"/>
+    </row>
+    <row r="11" spans="1:26" ht="42" x14ac:dyDescent="0.15">
       <c r="A11" s="8" t="s">
         <v>32</v>
       </c>
@@ -1048,31 +1149,31 @@
       <c r="D11" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
-      <c r="M11" s="6"/>
-      <c r="N11" s="6"/>
-      <c r="O11" s="6"/>
-      <c r="P11" s="6"/>
-      <c r="Q11" s="6"/>
-      <c r="R11" s="6"/>
-      <c r="S11" s="6"/>
-      <c r="T11" s="6"/>
-      <c r="U11" s="6"/>
-      <c r="V11" s="6"/>
-      <c r="W11" s="6"/>
-      <c r="X11" s="6"/>
-      <c r="Y11" s="6"/>
-      <c r="Z11" s="6"/>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A12" s="19" t="s">
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="8"/>
+      <c r="O11" s="8"/>
+      <c r="P11" s="8"/>
+      <c r="Q11" s="8"/>
+      <c r="R11" s="8"/>
+      <c r="S11" s="8"/>
+      <c r="T11" s="8"/>
+      <c r="U11" s="8"/>
+      <c r="V11" s="8"/>
+      <c r="W11" s="8"/>
+      <c r="X11" s="8"/>
+      <c r="Y11" s="8"/>
+      <c r="Z11" s="8"/>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.15">
+      <c r="A12" s="14" t="s">
         <v>36</v>
       </c>
       <c r="B12" s="17"/>
@@ -1101,7 +1202,7 @@
       <c r="Y12" s="17"/>
       <c r="Z12" s="17"/>
     </row>
-    <row r="13" spans="1:26" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:26" ht="84" x14ac:dyDescent="0.15">
       <c r="A13" s="8" t="s">
         <v>37</v>
       </c>
@@ -1114,30 +1215,30 @@
       <c r="D13" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="6"/>
-      <c r="M13" s="6"/>
-      <c r="N13" s="6"/>
-      <c r="O13" s="6"/>
-      <c r="P13" s="6"/>
-      <c r="Q13" s="6"/>
-      <c r="R13" s="6"/>
-      <c r="S13" s="6"/>
-      <c r="T13" s="6"/>
-      <c r="U13" s="6"/>
-      <c r="V13" s="6"/>
-      <c r="W13" s="6"/>
-      <c r="X13" s="6"/>
-      <c r="Y13" s="6"/>
-      <c r="Z13" s="6"/>
-    </row>
-    <row r="14" spans="1:26" ht="51" x14ac:dyDescent="0.2">
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8"/>
+      <c r="O13" s="8"/>
+      <c r="P13" s="8"/>
+      <c r="Q13" s="8"/>
+      <c r="R13" s="8"/>
+      <c r="S13" s="8"/>
+      <c r="T13" s="8"/>
+      <c r="U13" s="8"/>
+      <c r="V13" s="8"/>
+      <c r="W13" s="8"/>
+      <c r="X13" s="8"/>
+      <c r="Y13" s="8"/>
+      <c r="Z13" s="8"/>
+    </row>
+    <row r="14" spans="1:26" ht="56" x14ac:dyDescent="0.15">
       <c r="A14" s="8" t="s">
         <v>41</v>
       </c>
@@ -1150,30 +1251,30 @@
       <c r="D14" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="6"/>
-      <c r="M14" s="6"/>
-      <c r="N14" s="6"/>
-      <c r="O14" s="6"/>
-      <c r="P14" s="6"/>
-      <c r="Q14" s="6"/>
-      <c r="R14" s="6"/>
-      <c r="S14" s="6"/>
-      <c r="T14" s="6"/>
-      <c r="U14" s="6"/>
-      <c r="V14" s="6"/>
-      <c r="W14" s="6"/>
-      <c r="X14" s="6"/>
-      <c r="Y14" s="6"/>
-      <c r="Z14" s="6"/>
-    </row>
-    <row r="15" spans="1:26" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="8"/>
+      <c r="Q14" s="8"/>
+      <c r="R14" s="8"/>
+      <c r="S14" s="8"/>
+      <c r="T14" s="8"/>
+      <c r="U14" s="8"/>
+      <c r="V14" s="8"/>
+      <c r="W14" s="8"/>
+      <c r="X14" s="8"/>
+      <c r="Y14" s="8"/>
+      <c r="Z14" s="8"/>
+    </row>
+    <row r="15" spans="1:26" ht="70" x14ac:dyDescent="0.15">
       <c r="A15" s="8" t="s">
         <v>45</v>
       </c>
@@ -1186,30 +1287,30 @@
       <c r="D15" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
-      <c r="K15" s="6"/>
-      <c r="L15" s="6"/>
-      <c r="M15" s="6"/>
-      <c r="N15" s="6"/>
-      <c r="O15" s="6"/>
-      <c r="P15" s="6"/>
-      <c r="Q15" s="6"/>
-      <c r="R15" s="6"/>
-      <c r="S15" s="6"/>
-      <c r="T15" s="6"/>
-      <c r="U15" s="6"/>
-      <c r="V15" s="6"/>
-      <c r="W15" s="6"/>
-      <c r="X15" s="6"/>
-      <c r="Y15" s="6"/>
-      <c r="Z15" s="6"/>
-    </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="8"/>
+      <c r="O15" s="8"/>
+      <c r="P15" s="8"/>
+      <c r="Q15" s="8"/>
+      <c r="R15" s="8"/>
+      <c r="S15" s="8"/>
+      <c r="T15" s="8"/>
+      <c r="U15" s="8"/>
+      <c r="V15" s="8"/>
+      <c r="W15" s="8"/>
+      <c r="X15" s="8"/>
+      <c r="Y15" s="8"/>
+      <c r="Z15" s="8"/>
+    </row>
+    <row r="16" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A16" s="9" t="s">
         <v>49</v>
       </c>
@@ -1239,8 +1340,8 @@
       <c r="Y16" s="9"/>
       <c r="Z16" s="9"/>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A17" s="19" t="s">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.15">
+      <c r="A17" s="14" t="s">
         <v>50</v>
       </c>
       <c r="B17" s="17"/>
@@ -1269,7 +1370,7 @@
       <c r="Y17" s="17"/>
       <c r="Z17" s="17"/>
     </row>
-    <row r="18" spans="1:26" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:26" ht="42" x14ac:dyDescent="0.15">
       <c r="A18" s="8" t="s">
         <v>51</v>
       </c>
@@ -1282,30 +1383,30 @@
       <c r="D18" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="6"/>
-      <c r="K18" s="6"/>
-      <c r="L18" s="6"/>
-      <c r="M18" s="6"/>
-      <c r="N18" s="6"/>
-      <c r="O18" s="6"/>
-      <c r="P18" s="6"/>
-      <c r="Q18" s="6"/>
-      <c r="R18" s="6"/>
-      <c r="S18" s="6"/>
-      <c r="T18" s="6"/>
-      <c r="U18" s="6"/>
-      <c r="V18" s="6"/>
-      <c r="W18" s="6"/>
-      <c r="X18" s="6"/>
-      <c r="Y18" s="6"/>
-      <c r="Z18" s="6"/>
-    </row>
-    <row r="19" spans="1:26" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="8"/>
+      <c r="M18" s="8"/>
+      <c r="N18" s="8"/>
+      <c r="O18" s="8"/>
+      <c r="P18" s="8"/>
+      <c r="Q18" s="8"/>
+      <c r="R18" s="8"/>
+      <c r="S18" s="8"/>
+      <c r="T18" s="8"/>
+      <c r="U18" s="8"/>
+      <c r="V18" s="8"/>
+      <c r="W18" s="8"/>
+      <c r="X18" s="8"/>
+      <c r="Y18" s="8"/>
+      <c r="Z18" s="8"/>
+    </row>
+    <row r="19" spans="1:26" ht="70" x14ac:dyDescent="0.15">
       <c r="A19" s="8" t="s">
         <v>55</v>
       </c>
@@ -1318,30 +1419,30 @@
       <c r="D19" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="6"/>
-      <c r="L19" s="6"/>
-      <c r="M19" s="6"/>
-      <c r="N19" s="6"/>
-      <c r="O19" s="6"/>
-      <c r="P19" s="6"/>
-      <c r="Q19" s="6"/>
-      <c r="R19" s="6"/>
-      <c r="S19" s="6"/>
-      <c r="T19" s="6"/>
-      <c r="U19" s="6"/>
-      <c r="V19" s="6"/>
-      <c r="W19" s="6"/>
-      <c r="X19" s="6"/>
-      <c r="Y19" s="6"/>
-      <c r="Z19" s="6"/>
-    </row>
-    <row r="20" spans="1:26" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="8"/>
+      <c r="L19" s="8"/>
+      <c r="M19" s="8"/>
+      <c r="N19" s="8"/>
+      <c r="O19" s="8"/>
+      <c r="P19" s="8"/>
+      <c r="Q19" s="8"/>
+      <c r="R19" s="8"/>
+      <c r="S19" s="8"/>
+      <c r="T19" s="8"/>
+      <c r="U19" s="8"/>
+      <c r="V19" s="8"/>
+      <c r="W19" s="8"/>
+      <c r="X19" s="8"/>
+      <c r="Y19" s="8"/>
+      <c r="Z19" s="8"/>
+    </row>
+    <row r="20" spans="1:26" ht="70" x14ac:dyDescent="0.15">
       <c r="A20" s="8" t="s">
         <v>59</v>
       </c>
@@ -1354,30 +1455,30 @@
       <c r="D20" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="6"/>
-      <c r="L20" s="6"/>
-      <c r="M20" s="6"/>
-      <c r="N20" s="6"/>
-      <c r="O20" s="6"/>
-      <c r="P20" s="6"/>
-      <c r="Q20" s="6"/>
-      <c r="R20" s="6"/>
-      <c r="S20" s="6"/>
-      <c r="T20" s="6"/>
-      <c r="U20" s="6"/>
-      <c r="V20" s="6"/>
-      <c r="W20" s="6"/>
-      <c r="X20" s="6"/>
-      <c r="Y20" s="6"/>
-      <c r="Z20" s="6"/>
-    </row>
-    <row r="21" spans="1:26" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="8"/>
+      <c r="L20" s="8"/>
+      <c r="M20" s="8"/>
+      <c r="N20" s="8"/>
+      <c r="O20" s="8"/>
+      <c r="P20" s="8"/>
+      <c r="Q20" s="8"/>
+      <c r="R20" s="8"/>
+      <c r="S20" s="8"/>
+      <c r="T20" s="8"/>
+      <c r="U20" s="8"/>
+      <c r="V20" s="8"/>
+      <c r="W20" s="8"/>
+      <c r="X20" s="8"/>
+      <c r="Y20" s="8"/>
+      <c r="Z20" s="8"/>
+    </row>
+    <row r="21" spans="1:26" ht="70" x14ac:dyDescent="0.15">
       <c r="A21" s="8" t="s">
         <v>63</v>
       </c>
@@ -1390,60 +1491,60 @@
       <c r="D21" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
-      <c r="K21" s="6"/>
-      <c r="L21" s="6"/>
-      <c r="M21" s="6"/>
-      <c r="N21" s="6"/>
-      <c r="O21" s="6"/>
-      <c r="P21" s="6"/>
-      <c r="Q21" s="6"/>
-      <c r="R21" s="6"/>
-      <c r="S21" s="6"/>
-      <c r="T21" s="6"/>
-      <c r="U21" s="6"/>
-      <c r="V21" s="6"/>
-      <c r="W21" s="6"/>
-      <c r="X21" s="6"/>
-      <c r="Y21" s="6"/>
-      <c r="Z21" s="6"/>
-    </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A22" s="10" t="s">
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="8"/>
+      <c r="L21" s="8"/>
+      <c r="M21" s="8"/>
+      <c r="N21" s="8"/>
+      <c r="O21" s="8"/>
+      <c r="P21" s="8"/>
+      <c r="Q21" s="8"/>
+      <c r="R21" s="8"/>
+      <c r="S21" s="8"/>
+      <c r="T21" s="8"/>
+      <c r="U21" s="8"/>
+      <c r="V21" s="8"/>
+      <c r="W21" s="8"/>
+      <c r="X21" s="8"/>
+      <c r="Y21" s="8"/>
+      <c r="Z21" s="8"/>
+    </row>
+    <row r="22" spans="1:26" ht="14" x14ac:dyDescent="0.15">
+      <c r="A22" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="B22" s="11"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="12"/>
-      <c r="I22" s="12"/>
-      <c r="J22" s="12"/>
-      <c r="K22" s="12"/>
-      <c r="L22" s="12"/>
-      <c r="M22" s="12"/>
-      <c r="N22" s="12"/>
-      <c r="O22" s="12"/>
-      <c r="P22" s="12"/>
-      <c r="Q22" s="12"/>
-      <c r="R22" s="12"/>
-      <c r="S22" s="12"/>
-      <c r="T22" s="12"/>
-      <c r="U22" s="12"/>
-      <c r="V22" s="12"/>
-      <c r="W22" s="12"/>
-      <c r="X22" s="12"/>
-      <c r="Y22" s="12"/>
-      <c r="Z22" s="12"/>
-    </row>
-    <row r="23" spans="1:26" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="B22" s="18"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="19"/>
+      <c r="I22" s="19"/>
+      <c r="J22" s="19"/>
+      <c r="K22" s="19"/>
+      <c r="L22" s="19"/>
+      <c r="M22" s="19"/>
+      <c r="N22" s="19"/>
+      <c r="O22" s="19"/>
+      <c r="P22" s="19"/>
+      <c r="Q22" s="19"/>
+      <c r="R22" s="19"/>
+      <c r="S22" s="19"/>
+      <c r="T22" s="19"/>
+      <c r="U22" s="19"/>
+      <c r="V22" s="19"/>
+      <c r="W22" s="19"/>
+      <c r="X22" s="19"/>
+      <c r="Y22" s="19"/>
+      <c r="Z22" s="19"/>
+    </row>
+    <row r="23" spans="1:26" ht="84" x14ac:dyDescent="0.15">
       <c r="A23" s="8" t="s">
         <v>68</v>
       </c>
@@ -1456,8 +1557,30 @@
       <c r="D23" s="8" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="24" spans="1:26" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="16"/>
+      <c r="I23" s="16"/>
+      <c r="J23" s="16"/>
+      <c r="K23" s="16"/>
+      <c r="L23" s="16"/>
+      <c r="M23" s="16"/>
+      <c r="N23" s="16"/>
+      <c r="O23" s="16"/>
+      <c r="P23" s="16"/>
+      <c r="Q23" s="16"/>
+      <c r="R23" s="16"/>
+      <c r="S23" s="16"/>
+      <c r="T23" s="16"/>
+      <c r="U23" s="16"/>
+      <c r="V23" s="16"/>
+      <c r="W23" s="16"/>
+      <c r="X23" s="16"/>
+      <c r="Y23" s="16"/>
+      <c r="Z23" s="16"/>
+    </row>
+    <row r="24" spans="1:26" ht="70" x14ac:dyDescent="0.15">
       <c r="A24" s="8" t="s">
         <v>72</v>
       </c>
@@ -1470,8 +1593,30 @@
       <c r="D24" s="8" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="25" spans="1:26" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="16"/>
+      <c r="I24" s="16"/>
+      <c r="J24" s="16"/>
+      <c r="K24" s="16"/>
+      <c r="L24" s="16"/>
+      <c r="M24" s="16"/>
+      <c r="N24" s="16"/>
+      <c r="O24" s="16"/>
+      <c r="P24" s="16"/>
+      <c r="Q24" s="16"/>
+      <c r="R24" s="16"/>
+      <c r="S24" s="16"/>
+      <c r="T24" s="16"/>
+      <c r="U24" s="16"/>
+      <c r="V24" s="16"/>
+      <c r="W24" s="16"/>
+      <c r="X24" s="16"/>
+      <c r="Y24" s="16"/>
+      <c r="Z24" s="16"/>
+    </row>
+    <row r="25" spans="1:26" ht="70" x14ac:dyDescent="0.15">
       <c r="A25" s="8" t="s">
         <v>76</v>
       </c>
@@ -1484,8 +1629,30 @@
       <c r="D25" s="8" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="26" spans="1:26" ht="51" x14ac:dyDescent="0.2">
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="16"/>
+      <c r="I25" s="16"/>
+      <c r="J25" s="16"/>
+      <c r="K25" s="16"/>
+      <c r="L25" s="16"/>
+      <c r="M25" s="16"/>
+      <c r="N25" s="16"/>
+      <c r="O25" s="16"/>
+      <c r="P25" s="16"/>
+      <c r="Q25" s="16"/>
+      <c r="R25" s="16"/>
+      <c r="S25" s="16"/>
+      <c r="T25" s="16"/>
+      <c r="U25" s="16"/>
+      <c r="V25" s="16"/>
+      <c r="W25" s="16"/>
+      <c r="X25" s="16"/>
+      <c r="Y25" s="16"/>
+      <c r="Z25" s="16"/>
+    </row>
+    <row r="26" spans="1:26" ht="56" x14ac:dyDescent="0.15">
       <c r="A26" s="8" t="s">
         <v>80</v>
       </c>
@@ -1498,9 +1665,31 @@
       <c r="D26" s="8" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A27" s="18" t="s">
+      <c r="E26" s="16"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="16"/>
+      <c r="I26" s="16"/>
+      <c r="J26" s="16"/>
+      <c r="K26" s="16"/>
+      <c r="L26" s="16"/>
+      <c r="M26" s="16"/>
+      <c r="N26" s="16"/>
+      <c r="O26" s="16"/>
+      <c r="P26" s="16"/>
+      <c r="Q26" s="16"/>
+      <c r="R26" s="16"/>
+      <c r="S26" s="16"/>
+      <c r="T26" s="16"/>
+      <c r="U26" s="16"/>
+      <c r="V26" s="16"/>
+      <c r="W26" s="16"/>
+      <c r="X26" s="16"/>
+      <c r="Y26" s="16"/>
+      <c r="Z26" s="16"/>
+    </row>
+    <row r="27" spans="1:26" x14ac:dyDescent="0.15">
+      <c r="A27" s="20" t="s">
         <v>84</v>
       </c>
       <c r="B27" s="17"/>
@@ -1529,21 +1718,43 @@
       <c r="Y27" s="17"/>
       <c r="Z27" s="17"/>
     </row>
-    <row r="28" spans="1:26" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:26" ht="84" x14ac:dyDescent="0.15">
       <c r="A28" s="7" t="s">
         <v>85</v>
       </c>
       <c r="B28" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="C28" s="13" t="s">
+      <c r="C28" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="D28" s="13" t="s">
+      <c r="D28" s="7" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="29" spans="1:26" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="E28" s="16"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="16"/>
+      <c r="H28" s="16"/>
+      <c r="I28" s="16"/>
+      <c r="J28" s="16"/>
+      <c r="K28" s="16"/>
+      <c r="L28" s="16"/>
+      <c r="M28" s="16"/>
+      <c r="N28" s="16"/>
+      <c r="O28" s="16"/>
+      <c r="P28" s="16"/>
+      <c r="Q28" s="16"/>
+      <c r="R28" s="16"/>
+      <c r="S28" s="16"/>
+      <c r="T28" s="16"/>
+      <c r="U28" s="16"/>
+      <c r="V28" s="16"/>
+      <c r="W28" s="16"/>
+      <c r="X28" s="16"/>
+      <c r="Y28" s="16"/>
+      <c r="Z28" s="16"/>
+    </row>
+    <row r="29" spans="1:26" ht="84" x14ac:dyDescent="0.15">
       <c r="A29" s="7" t="s">
         <v>89</v>
       </c>
@@ -1556,39 +1767,61 @@
       <c r="D29" s="7" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A30" s="14" t="s">
+      <c r="E29" s="16"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="16"/>
+      <c r="H29" s="16"/>
+      <c r="I29" s="16"/>
+      <c r="J29" s="16"/>
+      <c r="K29" s="16"/>
+      <c r="L29" s="16"/>
+      <c r="M29" s="16"/>
+      <c r="N29" s="16"/>
+      <c r="O29" s="16"/>
+      <c r="P29" s="16"/>
+      <c r="Q29" s="16"/>
+      <c r="R29" s="16"/>
+      <c r="S29" s="16"/>
+      <c r="T29" s="16"/>
+      <c r="U29" s="16"/>
+      <c r="V29" s="16"/>
+      <c r="W29" s="16"/>
+      <c r="X29" s="16"/>
+      <c r="Y29" s="16"/>
+      <c r="Z29" s="16"/>
+    </row>
+    <row r="30" spans="1:26" ht="14" x14ac:dyDescent="0.15">
+      <c r="A30" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="B30" s="15"/>
-      <c r="C30" s="15"/>
-      <c r="D30" s="15"/>
-      <c r="E30" s="15"/>
-      <c r="F30" s="15"/>
-      <c r="G30" s="15"/>
-      <c r="H30" s="15"/>
-      <c r="I30" s="15"/>
-      <c r="J30" s="15"/>
-      <c r="K30" s="15"/>
-      <c r="L30" s="15"/>
-      <c r="M30" s="15"/>
-      <c r="N30" s="15"/>
-      <c r="O30" s="15"/>
-      <c r="P30" s="15"/>
-      <c r="Q30" s="15"/>
-      <c r="R30" s="15"/>
-      <c r="S30" s="15"/>
-      <c r="T30" s="15"/>
-      <c r="U30" s="15"/>
-      <c r="V30" s="15"/>
-      <c r="W30" s="15"/>
-      <c r="X30" s="15"/>
-      <c r="Y30" s="15"/>
-      <c r="Z30" s="15"/>
-    </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A31" s="19" t="s">
+      <c r="B30" s="10"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="10"/>
+      <c r="I30" s="10"/>
+      <c r="J30" s="10"/>
+      <c r="K30" s="10"/>
+      <c r="L30" s="10"/>
+      <c r="M30" s="10"/>
+      <c r="N30" s="10"/>
+      <c r="O30" s="10"/>
+      <c r="P30" s="10"/>
+      <c r="Q30" s="10"/>
+      <c r="R30" s="10"/>
+      <c r="S30" s="10"/>
+      <c r="T30" s="10"/>
+      <c r="U30" s="10"/>
+      <c r="V30" s="10"/>
+      <c r="W30" s="10"/>
+      <c r="X30" s="10"/>
+      <c r="Y30" s="10"/>
+      <c r="Z30" s="10"/>
+    </row>
+    <row r="31" spans="1:26" x14ac:dyDescent="0.15">
+      <c r="A31" s="14" t="s">
         <v>94</v>
       </c>
       <c r="B31" s="17"/>
@@ -1617,7 +1850,7 @@
       <c r="Y31" s="17"/>
       <c r="Z31" s="17"/>
     </row>
-    <row r="32" spans="1:26" ht="114.75" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:26" ht="112" x14ac:dyDescent="0.15">
       <c r="A32" s="8" t="s">
         <v>95</v>
       </c>
@@ -1630,30 +1863,30 @@
       <c r="D32" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="E32" s="6"/>
-      <c r="F32" s="6"/>
-      <c r="G32" s="6"/>
-      <c r="H32" s="6"/>
-      <c r="I32" s="6"/>
-      <c r="J32" s="6"/>
-      <c r="K32" s="6"/>
-      <c r="L32" s="6"/>
-      <c r="M32" s="6"/>
-      <c r="N32" s="6"/>
-      <c r="O32" s="6"/>
-      <c r="P32" s="6"/>
-      <c r="Q32" s="6"/>
-      <c r="R32" s="6"/>
-      <c r="S32" s="6"/>
-      <c r="T32" s="6"/>
-      <c r="U32" s="6"/>
-      <c r="V32" s="6"/>
-      <c r="W32" s="6"/>
-      <c r="X32" s="6"/>
-      <c r="Y32" s="6"/>
-      <c r="Z32" s="6"/>
-    </row>
-    <row r="33" spans="1:26" ht="102" x14ac:dyDescent="0.2">
+      <c r="E32" s="8"/>
+      <c r="F32" s="8"/>
+      <c r="G32" s="8"/>
+      <c r="H32" s="8"/>
+      <c r="I32" s="8"/>
+      <c r="J32" s="8"/>
+      <c r="K32" s="8"/>
+      <c r="L32" s="8"/>
+      <c r="M32" s="8"/>
+      <c r="N32" s="8"/>
+      <c r="O32" s="8"/>
+      <c r="P32" s="8"/>
+      <c r="Q32" s="8"/>
+      <c r="R32" s="8"/>
+      <c r="S32" s="8"/>
+      <c r="T32" s="8"/>
+      <c r="U32" s="8"/>
+      <c r="V32" s="8"/>
+      <c r="W32" s="8"/>
+      <c r="X32" s="8"/>
+      <c r="Y32" s="8"/>
+      <c r="Z32" s="8"/>
+    </row>
+    <row r="33" spans="1:26" ht="98" x14ac:dyDescent="0.15">
       <c r="A33" s="8" t="s">
         <v>99</v>
       </c>
@@ -1666,30 +1899,30 @@
       <c r="D33" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="E33" s="6"/>
-      <c r="F33" s="6"/>
-      <c r="G33" s="6"/>
-      <c r="H33" s="6"/>
-      <c r="I33" s="6"/>
-      <c r="J33" s="6"/>
-      <c r="K33" s="6"/>
-      <c r="L33" s="6"/>
-      <c r="M33" s="6"/>
-      <c r="N33" s="6"/>
-      <c r="O33" s="6"/>
-      <c r="P33" s="6"/>
-      <c r="Q33" s="6"/>
-      <c r="R33" s="6"/>
-      <c r="S33" s="6"/>
-      <c r="T33" s="6"/>
-      <c r="U33" s="6"/>
-      <c r="V33" s="6"/>
-      <c r="W33" s="6"/>
-      <c r="X33" s="6"/>
-      <c r="Y33" s="6"/>
-      <c r="Z33" s="6"/>
-    </row>
-    <row r="34" spans="1:26" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="E33" s="8"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="8"/>
+      <c r="H33" s="8"/>
+      <c r="I33" s="8"/>
+      <c r="J33" s="8"/>
+      <c r="K33" s="8"/>
+      <c r="L33" s="8"/>
+      <c r="M33" s="8"/>
+      <c r="N33" s="8"/>
+      <c r="O33" s="8"/>
+      <c r="P33" s="8"/>
+      <c r="Q33" s="8"/>
+      <c r="R33" s="8"/>
+      <c r="S33" s="8"/>
+      <c r="T33" s="8"/>
+      <c r="U33" s="8"/>
+      <c r="V33" s="8"/>
+      <c r="W33" s="8"/>
+      <c r="X33" s="8"/>
+      <c r="Y33" s="8"/>
+      <c r="Z33" s="8"/>
+    </row>
+    <row r="34" spans="1:26" ht="98" x14ac:dyDescent="0.15">
       <c r="A34" s="8" t="s">
         <v>103</v>
       </c>
@@ -1702,31 +1935,31 @@
       <c r="D34" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="E34" s="6"/>
-      <c r="F34" s="6"/>
-      <c r="G34" s="6"/>
-      <c r="H34" s="6"/>
-      <c r="I34" s="6"/>
-      <c r="J34" s="6"/>
-      <c r="K34" s="6"/>
-      <c r="L34" s="6"/>
-      <c r="M34" s="6"/>
-      <c r="N34" s="6"/>
-      <c r="O34" s="6"/>
-      <c r="P34" s="6"/>
-      <c r="Q34" s="6"/>
-      <c r="R34" s="6"/>
-      <c r="S34" s="6"/>
-      <c r="T34" s="6"/>
-      <c r="U34" s="6"/>
-      <c r="V34" s="6"/>
-      <c r="W34" s="6"/>
-      <c r="X34" s="6"/>
-      <c r="Y34" s="6"/>
-      <c r="Z34" s="6"/>
-    </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A35" s="19" t="s">
+      <c r="E34" s="8"/>
+      <c r="F34" s="8"/>
+      <c r="G34" s="8"/>
+      <c r="H34" s="8"/>
+      <c r="I34" s="8"/>
+      <c r="J34" s="8"/>
+      <c r="K34" s="8"/>
+      <c r="L34" s="8"/>
+      <c r="M34" s="8"/>
+      <c r="N34" s="8"/>
+      <c r="O34" s="8"/>
+      <c r="P34" s="8"/>
+      <c r="Q34" s="8"/>
+      <c r="R34" s="8"/>
+      <c r="S34" s="8"/>
+      <c r="T34" s="8"/>
+      <c r="U34" s="8"/>
+      <c r="V34" s="8"/>
+      <c r="W34" s="8"/>
+      <c r="X34" s="8"/>
+      <c r="Y34" s="8"/>
+      <c r="Z34" s="8"/>
+    </row>
+    <row r="35" spans="1:26" x14ac:dyDescent="0.15">
+      <c r="A35" s="14" t="s">
         <v>107</v>
       </c>
       <c r="B35" s="17"/>
@@ -1755,7 +1988,7 @@
       <c r="Y35" s="17"/>
       <c r="Z35" s="17"/>
     </row>
-    <row r="36" spans="1:26" ht="127.5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:26" ht="140" x14ac:dyDescent="0.15">
       <c r="A36" s="8" t="s">
         <v>108</v>
       </c>
@@ -1768,30 +2001,30 @@
       <c r="D36" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="E36" s="6"/>
-      <c r="F36" s="6"/>
-      <c r="G36" s="6"/>
-      <c r="H36" s="6"/>
-      <c r="I36" s="6"/>
-      <c r="J36" s="6"/>
-      <c r="K36" s="6"/>
-      <c r="L36" s="6"/>
-      <c r="M36" s="6"/>
-      <c r="N36" s="6"/>
-      <c r="O36" s="6"/>
-      <c r="P36" s="6"/>
-      <c r="Q36" s="6"/>
-      <c r="R36" s="6"/>
-      <c r="S36" s="6"/>
-      <c r="T36" s="6"/>
-      <c r="U36" s="6"/>
-      <c r="V36" s="6"/>
-      <c r="W36" s="6"/>
-      <c r="X36" s="6"/>
-      <c r="Y36" s="6"/>
-      <c r="Z36" s="6"/>
-    </row>
-    <row r="37" spans="1:26" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="E36" s="8"/>
+      <c r="F36" s="8"/>
+      <c r="G36" s="8"/>
+      <c r="H36" s="8"/>
+      <c r="I36" s="8"/>
+      <c r="J36" s="8"/>
+      <c r="K36" s="8"/>
+      <c r="L36" s="8"/>
+      <c r="M36" s="8"/>
+      <c r="N36" s="8"/>
+      <c r="O36" s="8"/>
+      <c r="P36" s="8"/>
+      <c r="Q36" s="8"/>
+      <c r="R36" s="8"/>
+      <c r="S36" s="8"/>
+      <c r="T36" s="8"/>
+      <c r="U36" s="8"/>
+      <c r="V36" s="8"/>
+      <c r="W36" s="8"/>
+      <c r="X36" s="8"/>
+      <c r="Y36" s="8"/>
+      <c r="Z36" s="8"/>
+    </row>
+    <row r="37" spans="1:26" ht="84" x14ac:dyDescent="0.15">
       <c r="A37" s="8" t="s">
         <v>112</v>
       </c>
@@ -1804,30 +2037,30 @@
       <c r="D37" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="E37" s="6"/>
-      <c r="F37" s="6"/>
-      <c r="G37" s="6"/>
-      <c r="H37" s="6"/>
-      <c r="I37" s="6"/>
-      <c r="J37" s="6"/>
-      <c r="K37" s="6"/>
-      <c r="L37" s="6"/>
-      <c r="M37" s="6"/>
-      <c r="N37" s="6"/>
-      <c r="O37" s="6"/>
-      <c r="P37" s="6"/>
-      <c r="Q37" s="6"/>
-      <c r="R37" s="6"/>
-      <c r="S37" s="6"/>
-      <c r="T37" s="6"/>
-      <c r="U37" s="6"/>
-      <c r="V37" s="6"/>
-      <c r="W37" s="6"/>
-      <c r="X37" s="6"/>
-      <c r="Y37" s="6"/>
-      <c r="Z37" s="6"/>
-    </row>
-    <row r="38" spans="1:26" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="E37" s="8"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="8"/>
+      <c r="H37" s="8"/>
+      <c r="I37" s="8"/>
+      <c r="J37" s="8"/>
+      <c r="K37" s="8"/>
+      <c r="L37" s="8"/>
+      <c r="M37" s="8"/>
+      <c r="N37" s="8"/>
+      <c r="O37" s="8"/>
+      <c r="P37" s="8"/>
+      <c r="Q37" s="8"/>
+      <c r="R37" s="8"/>
+      <c r="S37" s="8"/>
+      <c r="T37" s="8"/>
+      <c r="U37" s="8"/>
+      <c r="V37" s="8"/>
+      <c r="W37" s="8"/>
+      <c r="X37" s="8"/>
+      <c r="Y37" s="8"/>
+      <c r="Z37" s="8"/>
+    </row>
+    <row r="38" spans="1:26" ht="84" x14ac:dyDescent="0.15">
       <c r="A38" s="8" t="s">
         <v>116</v>
       </c>
@@ -1840,28 +2073,28 @@
       <c r="D38" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="E38" s="6"/>
-      <c r="F38" s="6"/>
-      <c r="G38" s="6"/>
-      <c r="H38" s="6"/>
-      <c r="I38" s="6"/>
-      <c r="J38" s="6"/>
-      <c r="K38" s="6"/>
-      <c r="L38" s="6"/>
-      <c r="M38" s="6"/>
-      <c r="N38" s="6"/>
-      <c r="O38" s="6"/>
-      <c r="P38" s="6"/>
-      <c r="Q38" s="6"/>
-      <c r="R38" s="6"/>
-      <c r="S38" s="6"/>
-      <c r="T38" s="6"/>
-      <c r="U38" s="6"/>
-      <c r="V38" s="6"/>
-      <c r="W38" s="6"/>
-      <c r="X38" s="6"/>
-      <c r="Y38" s="6"/>
-      <c r="Z38" s="6"/>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="8"/>
+      <c r="H38" s="8"/>
+      <c r="I38" s="8"/>
+      <c r="J38" s="8"/>
+      <c r="K38" s="8"/>
+      <c r="L38" s="8"/>
+      <c r="M38" s="8"/>
+      <c r="N38" s="8"/>
+      <c r="O38" s="8"/>
+      <c r="P38" s="8"/>
+      <c r="Q38" s="8"/>
+      <c r="R38" s="8"/>
+      <c r="S38" s="8"/>
+      <c r="T38" s="8"/>
+      <c r="U38" s="8"/>
+      <c r="V38" s="8"/>
+      <c r="W38" s="8"/>
+      <c r="X38" s="8"/>
+      <c r="Y38" s="8"/>
+      <c r="Z38" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -1876,7 +2109,7 @@
   </mergeCells>
   <printOptions horizontalCentered="1" gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup scale="71" fitToHeight="0" pageOrder="overThenDown" orientation="landscape" cellComments="atEnd" r:id="rId1"/>
+  <pageSetup scale="65" fitToHeight="0" pageOrder="overThenDown" orientation="landscape" cellComments="atEnd" r:id="rId1"/>
   <rowBreaks count="1" manualBreakCount="1">
     <brk id="15" max="3" man="1"/>
   </rowBreaks>

</xml_diff>